<commit_message>
-mis à jour le colloscope
</commit_message>
<xml_diff>
--- a/assets/colloscope.xlsx
+++ b/assets/colloscope.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f027f7f3b6b568fb/Documents/Boulot/MP2I_23_24/Colles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\colloscope\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{A75E52C6-51E8-4E3D-A16A-D410FFFEBAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{540E5BE0-1789-4A88-BBA2-737F83EC0176}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A358F3-1793-4A86-9216-56A0C8F410A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-5520" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Colloscope_MP2I_2324_Semestre_1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="244">
   <si>
     <t>Étudiant 1</t>
   </si>
@@ -877,13 +877,16 @@
     </r>
   </si>
   <si>
-    <t>B204</t>
-  </si>
-  <si>
     <t>Lundi 12h45</t>
   </si>
   <si>
     <t>Vendredi 12h45</t>
+  </si>
+  <si>
+    <t>B113</t>
+  </si>
+  <si>
+    <t>B301</t>
   </si>
 </sst>
 </file>
@@ -2655,21 +2658,21 @@
   </sheetPr>
   <dimension ref="A1:AM55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="22" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="140" t="s">
         <v>66</v>
       </c>
@@ -2695,7 +2698,7 @@
       <c r="U1" s="141"/>
       <c r="V1" s="142"/>
     </row>
-    <row r="2" spans="1:36" s="25" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" s="25" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="143"/>
       <c r="B2" s="144"/>
       <c r="C2" s="144"/>
@@ -2719,7 +2722,7 @@
       <c r="U2" s="144"/>
       <c r="V2" s="145"/>
     </row>
-    <row r="3" spans="1:36" s="25" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" s="25" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="143"/>
       <c r="B3" s="144"/>
       <c r="C3" s="144"/>
@@ -2743,7 +2746,7 @@
       <c r="U3" s="144"/>
       <c r="V3" s="145"/>
     </row>
-    <row r="4" spans="1:36" s="25" customFormat="1" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" s="25" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="146"/>
       <c r="B4" s="147"/>
       <c r="C4" s="147"/>
@@ -2767,7 +2770,7 @@
       <c r="U4" s="147"/>
       <c r="V4" s="148"/>
     </row>
-    <row r="5" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2793,7 +2796,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:36" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2821,7 +2824,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:36" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="152"/>
@@ -2846,7 +2849,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="134" t="s">
         <v>67</v>
       </c>
@@ -2906,7 +2909,7 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
-    <row r="9" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="137"/>
       <c r="B9" s="138"/>
       <c r="C9" s="138"/>
@@ -2966,7 +2969,7 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
     </row>
-    <row r="10" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>137</v>
       </c>
@@ -3035,7 +3038,7 @@
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
     </row>
-    <row r="11" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
         <v>138</v>
       </c>
@@ -3115,7 +3118,7 @@
       <c r="AI11" s="5"/>
       <c r="AJ11" s="5"/>
     </row>
-    <row r="12" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="39" t="s">
         <v>139</v>
       </c>
@@ -3195,7 +3198,7 @@
       <c r="AI12" s="5"/>
       <c r="AJ12" s="5"/>
     </row>
-    <row r="13" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
         <v>140</v>
       </c>
@@ -3275,7 +3278,7 @@
       <c r="AI13" s="5"/>
       <c r="AJ13" s="5"/>
     </row>
-    <row r="14" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="39" t="s">
         <v>141</v>
       </c>
@@ -3355,7 +3358,7 @@
       <c r="AI14" s="5"/>
       <c r="AJ14" s="5"/>
     </row>
-    <row r="15" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
         <v>142</v>
       </c>
@@ -3435,7 +3438,7 @@
       <c r="AI15" s="5"/>
       <c r="AJ15" s="5"/>
     </row>
-    <row r="16" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
         <v>143</v>
       </c>
@@ -3515,7 +3518,7 @@
       <c r="AI16" s="5"/>
       <c r="AJ16" s="5"/>
     </row>
-    <row r="17" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
         <v>144</v>
       </c>
@@ -3595,7 +3598,7 @@
       <c r="AI17" s="5"/>
       <c r="AJ17" s="5"/>
     </row>
-    <row r="18" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
         <v>145</v>
       </c>
@@ -3675,7 +3678,7 @@
       <c r="AI18" s="5"/>
       <c r="AJ18" s="5"/>
     </row>
-    <row r="19" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
         <v>146</v>
       </c>
@@ -3755,7 +3758,7 @@
       <c r="AI19" s="5"/>
       <c r="AJ19" s="5"/>
     </row>
-    <row r="20" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
         <v>147</v>
       </c>
@@ -3835,7 +3838,7 @@
       <c r="AI20" s="5"/>
       <c r="AJ20" s="5"/>
     </row>
-    <row r="21" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="39" t="s">
         <v>148</v>
       </c>
@@ -3915,7 +3918,7 @@
       <c r="AI21" s="5"/>
       <c r="AJ21" s="5"/>
     </row>
-    <row r="22" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="39" t="s">
         <v>149</v>
       </c>
@@ -3995,7 +3998,7 @@
       <c r="AI22" s="5"/>
       <c r="AJ22" s="5"/>
     </row>
-    <row r="23" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>150</v>
       </c>
@@ -4075,7 +4078,7 @@
       <c r="AI23" s="5"/>
       <c r="AJ23" s="5"/>
     </row>
-    <row r="24" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>151</v>
       </c>
@@ -4155,7 +4158,7 @@
       <c r="AI24" s="5"/>
       <c r="AJ24" s="5"/>
     </row>
-    <row r="25" spans="1:39" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="44" t="s">
         <v>152</v>
       </c>
@@ -4235,7 +4238,7 @@
       <c r="AI25" s="5"/>
       <c r="AJ25" s="5"/>
     </row>
-    <row r="26" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D26" s="20"/>
       <c r="E26" s="2"/>
       <c r="X26" s="1"/>
@@ -4255,7 +4258,7 @@
       <c r="AL26" s="5"/>
       <c r="AM26" s="5"/>
     </row>
-    <row r="27" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D27" s="20"/>
       <c r="E27" s="2"/>
       <c r="X27" s="1"/>
@@ -4275,7 +4278,7 @@
       <c r="AL27" s="5"/>
       <c r="AM27" s="5"/>
     </row>
-    <row r="28" spans="1:39" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="20"/>
       <c r="E28" s="2"/>
       <c r="X28" s="5"/>
@@ -4289,7 +4292,7 @@
       <c r="AF28" s="5"/>
       <c r="AG28" s="5"/>
     </row>
-    <row r="29" spans="1:39" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="134" t="s">
         <v>205</v>
       </c>
@@ -4314,7 +4317,7 @@
       <c r="T29" s="135"/>
       <c r="U29" s="136"/>
     </row>
-    <row r="30" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="137"/>
       <c r="C30" s="138"/>
       <c r="D30" s="138"/>
@@ -4333,7 +4336,7 @@
       <c r="T30" s="138"/>
       <c r="U30" s="139"/>
     </row>
-    <row r="31" spans="1:39" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:39" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="31"/>
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
@@ -4368,7 +4371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="163" t="s">
         <v>206</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="53"/>
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
@@ -4440,7 +4443,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="163" t="s">
         <v>230</v>
       </c>
@@ -4477,7 +4480,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="163"/>
       <c r="C35" s="164"/>
       <c r="D35" s="164"/>
@@ -4487,14 +4490,14 @@
       </c>
       <c r="I35" s="69"/>
       <c r="J35" s="70" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="K35" s="71"/>
       <c r="L35" s="72" t="s">
         <v>103</v>
       </c>
       <c r="M35" s="73" t="s">
-        <v>115</v>
+        <v>242</v>
       </c>
       <c r="O35" s="91"/>
       <c r="P35" s="85" t="s">
@@ -4512,7 +4515,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="53"/>
       <c r="C36" s="54"/>
       <c r="D36" s="54"/>
@@ -4547,7 +4550,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="163" t="s">
         <v>213</v>
       </c>
@@ -4584,7 +4587,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="163"/>
       <c r="C38" s="164"/>
       <c r="D38" s="164"/>
@@ -4619,7 +4622,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="2:21" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:21" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="56"/>
       <c r="C39" s="57"/>
       <c r="D39" s="57"/>
@@ -4654,7 +4657,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="2:21" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="163" t="s">
         <v>212</v>
       </c>
@@ -4685,7 +4688,7 @@
       <c r="T40" s="135"/>
       <c r="U40" s="136"/>
     </row>
-    <row r="41" spans="2:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="163"/>
       <c r="C41" s="164"/>
       <c r="D41" s="164"/>
@@ -4702,7 +4705,7 @@
         <v>109</v>
       </c>
       <c r="M41" s="73" t="s">
-        <v>115</v>
+        <v>242</v>
       </c>
       <c r="O41" s="105"/>
       <c r="P41" s="137"/>
@@ -4712,7 +4715,7 @@
       <c r="T41" s="138"/>
       <c r="U41" s="139"/>
     </row>
-    <row r="42" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="59"/>
       <c r="C42" s="60"/>
       <c r="D42" s="60"/>
@@ -4747,7 +4750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="2:21" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:21" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H43" s="75" t="s">
         <v>8</v>
       </c>
@@ -4778,7 +4781,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="44" spans="2:21" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H44" s="134" t="s">
         <v>159</v>
       </c>
@@ -4803,7 +4806,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="2:21" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:21" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H45" s="137"/>
       <c r="I45" s="138"/>
       <c r="J45" s="138"/>
@@ -4826,7 +4829,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="2:21" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:21" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="155" t="s">
         <v>202</v>
       </c>
@@ -4863,7 +4866,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="158"/>
       <c r="C47" s="159"/>
       <c r="D47" s="159"/>
@@ -4895,10 +4898,10 @@
         <v>85</v>
       </c>
       <c r="U47" s="88" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="48" spans="2:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="26" t="s">
         <v>3</v>
       </c>
@@ -4914,7 +4917,7 @@
       </c>
       <c r="I48" s="98"/>
       <c r="J48" s="70" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K48" s="71"/>
       <c r="L48" s="72" t="s">
@@ -4939,7 +4942,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="49" spans="2:24" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="62" t="s">
         <v>68</v>
       </c>
@@ -4983,7 +4986,7 @@
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
     </row>
-    <row r="50" spans="2:24" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="99" t="s">
         <v>68</v>
       </c>
@@ -5001,7 +5004,7 @@
       </c>
       <c r="I50" s="100"/>
       <c r="J50" s="101" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K50" s="102"/>
       <c r="L50" s="103" t="s">
@@ -5029,7 +5032,7 @@
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
     </row>
-    <row r="51" spans="2:24" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:24" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
@@ -5043,34 +5046,34 @@
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
     </row>
-    <row r="52" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:24" x14ac:dyDescent="0.25">
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:24" x14ac:dyDescent="0.25">
       <c r="Q53" s="1"/>
     </row>
-    <row r="55" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:24" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
       <c r="X55" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="H44:M45"/>
+    <mergeCell ref="B46:E47"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="B34:E35"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B37:E38"/>
+    <mergeCell ref="B40:E41"/>
     <mergeCell ref="P29:U30"/>
     <mergeCell ref="P40:U41"/>
     <mergeCell ref="A8:D9"/>
     <mergeCell ref="A1:V4"/>
     <mergeCell ref="G6:V7"/>
     <mergeCell ref="H29:M30"/>
-    <mergeCell ref="H44:M45"/>
-    <mergeCell ref="B46:E47"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="B34:E35"/>
-    <mergeCell ref="C50:D50"/>
     <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B37:E38"/>
-    <mergeCell ref="B40:E41"/>
     <mergeCell ref="B29:E30"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
@@ -5088,12 +5091,12 @@
       <selection sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="12.21875" customWidth="1"/>
+    <col min="2" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="168" t="s">
         <v>64</v>
       </c>
@@ -5101,7 +5104,7 @@
       <c r="C1" s="168"/>
       <c r="D1" s="168"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>65</v>
       </c>
@@ -5115,7 +5118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -5129,7 +5132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -5143,7 +5146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -5157,7 +5160,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -5171,7 +5174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -5185,7 +5188,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -5199,7 +5202,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -5213,7 +5216,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -5227,7 +5230,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -5241,7 +5244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -5255,7 +5258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -5269,7 +5272,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -5281,7 +5284,7 @@
       </c>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -5295,7 +5298,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -5309,7 +5312,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -5323,7 +5326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>16</v>
       </c>
@@ -5337,7 +5340,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
-mis à jour pour les colles d'info
</commit_message>
<xml_diff>
--- a/assets/colloscope.xlsx
+++ b/assets/colloscope.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\colloscope\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A051AB-AB96-450B-B20A-003409CD1FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121AF102-36D0-4E7B-9CA3-3325D16E6F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Colloscope_MP2I_2324_Semestre_1" sheetId="1" r:id="rId1"/>
@@ -738,9 +738,6 @@
     <t>I3 +  P4</t>
   </si>
   <si>
-    <t>Vendredi 15h30</t>
-  </si>
-  <si>
     <t>M. Paparazzo</t>
   </si>
   <si>
@@ -814,6 +811,9 @@
       </rPr>
       <t>LE MELINAIDRE</t>
     </r>
+  </si>
+  <si>
+    <t>Vendredi 15h15</t>
   </si>
 </sst>
 </file>
@@ -2049,7 +2049,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2230,6 +2230,315 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2248,22 +2557,49 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2275,419 +2611,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2921,8 +2864,8 @@
   </sheetPr>
   <dimension ref="A1:AM55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,102 +2879,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="175" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="83"/>
+      <c r="B1" s="176"/>
+      <c r="C1" s="176"/>
+      <c r="D1" s="176"/>
+      <c r="E1" s="176"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
+      <c r="O1" s="176"/>
+      <c r="P1" s="176"/>
+      <c r="Q1" s="176"/>
+      <c r="R1" s="176"/>
+      <c r="S1" s="176"/>
+      <c r="T1" s="176"/>
+      <c r="U1" s="176"/>
+      <c r="V1" s="177"/>
     </row>
     <row r="2" spans="1:36" s="25" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="86"/>
+      <c r="A2" s="178"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
+      <c r="H2" s="179"/>
+      <c r="I2" s="179"/>
+      <c r="J2" s="179"/>
+      <c r="K2" s="179"/>
+      <c r="L2" s="179"/>
+      <c r="M2" s="179"/>
+      <c r="N2" s="179"/>
+      <c r="O2" s="179"/>
+      <c r="P2" s="179"/>
+      <c r="Q2" s="179"/>
+      <c r="R2" s="179"/>
+      <c r="S2" s="179"/>
+      <c r="T2" s="179"/>
+      <c r="U2" s="179"/>
+      <c r="V2" s="180"/>
     </row>
     <row r="3" spans="1:36" s="25" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84"/>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="86"/>
+      <c r="A3" s="178"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="179"/>
+      <c r="O3" s="179"/>
+      <c r="P3" s="179"/>
+      <c r="Q3" s="179"/>
+      <c r="R3" s="179"/>
+      <c r="S3" s="179"/>
+      <c r="T3" s="179"/>
+      <c r="U3" s="179"/>
+      <c r="V3" s="180"/>
     </row>
     <row r="4" spans="1:36" s="25" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="89"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="182"/>
+      <c r="C4" s="182"/>
+      <c r="D4" s="182"/>
+      <c r="E4" s="182"/>
+      <c r="F4" s="182"/>
+      <c r="G4" s="182"/>
+      <c r="H4" s="182"/>
+      <c r="I4" s="182"/>
+      <c r="J4" s="182"/>
+      <c r="K4" s="182"/>
+      <c r="L4" s="182"/>
+      <c r="M4" s="182"/>
+      <c r="N4" s="182"/>
+      <c r="O4" s="182"/>
+      <c r="P4" s="182"/>
+      <c r="Q4" s="182"/>
+      <c r="R4" s="182"/>
+      <c r="S4" s="182"/>
+      <c r="T4" s="182"/>
+      <c r="U4" s="182"/>
+      <c r="V4" s="183"/>
     </row>
     <row r="5" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
@@ -3063,24 +3006,24 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="90" t="s">
+      <c r="G6" s="184" t="s">
         <v>200</v>
       </c>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="91"/>
-      <c r="S6" s="91"/>
-      <c r="T6" s="91"/>
-      <c r="U6" s="91"/>
-      <c r="V6" s="92"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="185"/>
+      <c r="K6" s="185"/>
+      <c r="L6" s="185"/>
+      <c r="M6" s="185"/>
+      <c r="N6" s="185"/>
+      <c r="O6" s="185"/>
+      <c r="P6" s="185"/>
+      <c r="Q6" s="185"/>
+      <c r="R6" s="185"/>
+      <c r="S6" s="185"/>
+      <c r="T6" s="185"/>
+      <c r="U6" s="185"/>
+      <c r="V6" s="186"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -3090,22 +3033,22 @@
     <row r="7" spans="1:36" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="94"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="94"/>
-      <c r="U7" s="94"/>
-      <c r="V7" s="95"/>
+      <c r="G7" s="187"/>
+      <c r="H7" s="188"/>
+      <c r="I7" s="188"/>
+      <c r="J7" s="188"/>
+      <c r="K7" s="188"/>
+      <c r="L7" s="188"/>
+      <c r="M7" s="188"/>
+      <c r="N7" s="188"/>
+      <c r="O7" s="188"/>
+      <c r="P7" s="188"/>
+      <c r="Q7" s="188"/>
+      <c r="R7" s="188"/>
+      <c r="S7" s="188"/>
+      <c r="T7" s="188"/>
+      <c r="U7" s="188"/>
+      <c r="V7" s="189"/>
       <c r="W7" s="21"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -3113,54 +3056,54 @@
       <c r="AA7" s="1"/>
     </row>
     <row r="8" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="169" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
+      <c r="B8" s="170"/>
+      <c r="C8" s="170"/>
+      <c r="D8" s="171"/>
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="98">
+      <c r="G8" s="67">
         <v>45334</v>
       </c>
-      <c r="H8" s="99">
+      <c r="H8" s="68">
         <v>45341</v>
       </c>
-      <c r="I8" s="100">
+      <c r="I8" s="69">
         <v>45362</v>
       </c>
-      <c r="J8" s="101">
+      <c r="J8" s="70">
         <v>45369</v>
       </c>
-      <c r="K8" s="101">
+      <c r="K8" s="70">
         <v>45376</v>
       </c>
-      <c r="L8" s="101">
+      <c r="L8" s="70">
         <v>45383</v>
       </c>
-      <c r="M8" s="101">
+      <c r="M8" s="70">
         <v>45390</v>
       </c>
-      <c r="N8" s="99">
+      <c r="N8" s="68">
         <v>45397</v>
       </c>
-      <c r="O8" s="100">
+      <c r="O8" s="69">
         <v>45425</v>
       </c>
-      <c r="P8" s="101">
+      <c r="P8" s="70">
         <v>45432</v>
       </c>
-      <c r="Q8" s="101">
+      <c r="Q8" s="70">
         <v>45439</v>
       </c>
-      <c r="R8" s="101">
+      <c r="R8" s="70">
         <v>45446</v>
       </c>
-      <c r="S8" s="102">
+      <c r="S8" s="71">
         <v>45453</v>
       </c>
-      <c r="T8" s="103">
+      <c r="T8" s="72">
         <v>45460</v>
       </c>
       <c r="U8" s="40"/>
@@ -3169,54 +3112,54 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="69"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="71"/>
+      <c r="A9" s="172"/>
+      <c r="B9" s="173"/>
+      <c r="C9" s="173"/>
+      <c r="D9" s="174"/>
       <c r="E9" s="3"/>
       <c r="F9" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="G9" s="104">
+      <c r="G9" s="73">
         <v>17</v>
       </c>
-      <c r="H9" s="105">
+      <c r="H9" s="74">
         <v>18</v>
       </c>
-      <c r="I9" s="106">
+      <c r="I9" s="75">
         <v>19</v>
       </c>
-      <c r="J9" s="107">
+      <c r="J9" s="76">
         <v>20</v>
       </c>
-      <c r="K9" s="107">
+      <c r="K9" s="76">
         <v>21</v>
       </c>
-      <c r="L9" s="108">
+      <c r="L9" s="77">
         <v>22</v>
       </c>
-      <c r="M9" s="108">
+      <c r="M9" s="77">
         <v>23</v>
       </c>
-      <c r="N9" s="109">
+      <c r="N9" s="78">
         <v>24</v>
       </c>
-      <c r="O9" s="106">
+      <c r="O9" s="75">
         <v>25</v>
       </c>
-      <c r="P9" s="108">
+      <c r="P9" s="77">
         <v>26</v>
       </c>
-      <c r="Q9" s="107">
+      <c r="Q9" s="76">
         <v>27</v>
       </c>
-      <c r="R9" s="106">
+      <c r="R9" s="75">
         <v>28</v>
       </c>
-      <c r="S9" s="108">
+      <c r="S9" s="77">
         <v>29</v>
       </c>
-      <c r="T9" s="110">
+      <c r="T9" s="79">
         <v>30</v>
       </c>
       <c r="U9" s="56"/>
@@ -3228,59 +3171,59 @@
       <c r="A10" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="151" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="208" t="s">
+      <c r="C10" s="152" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="209" t="s">
+      <c r="D10" s="153" t="s">
         <v>132</v>
       </c>
       <c r="E10" s="34"/>
       <c r="F10" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="G10" s="111" t="s">
+      <c r="G10" s="80" t="s">
         <v>207</v>
       </c>
-      <c r="H10" s="112" t="s">
+      <c r="H10" s="81" t="s">
         <v>227</v>
       </c>
-      <c r="I10" s="113" t="s">
+      <c r="I10" s="82" t="s">
         <v>215</v>
       </c>
-      <c r="J10" s="114" t="s">
+      <c r="J10" s="83" t="s">
         <v>214</v>
       </c>
-      <c r="K10" s="114" t="s">
+      <c r="K10" s="83" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="114" t="s">
+      <c r="L10" s="83" t="s">
         <v>228</v>
       </c>
-      <c r="M10" s="128" t="s">
+      <c r="M10" s="97" t="s">
         <v>220</v>
       </c>
-      <c r="N10" s="112" t="s">
+      <c r="N10" s="81" t="s">
         <v>218</v>
       </c>
-      <c r="O10" s="113" t="s">
+      <c r="O10" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="P10" s="114" t="s">
+      <c r="P10" s="83" t="s">
         <v>211</v>
       </c>
-      <c r="Q10" s="114" t="s">
+      <c r="Q10" s="83" t="s">
         <v>210</v>
       </c>
-      <c r="R10" s="114" t="s">
+      <c r="R10" s="83" t="s">
         <v>229</v>
       </c>
-      <c r="S10" s="114" t="s">
+      <c r="S10" s="83" t="s">
         <v>221</v>
       </c>
-      <c r="T10" s="127" t="s">
+      <c r="T10" s="96" t="s">
         <v>230</v>
       </c>
       <c r="U10" s="58"/>
@@ -3293,59 +3236,59 @@
       <c r="A11" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="210" t="s">
+      <c r="B11" s="154" t="s">
         <v>149</v>
       </c>
-      <c r="C11" s="211" t="s">
+      <c r="C11" s="155" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="212" t="s">
+      <c r="D11" s="156" t="s">
         <v>151</v>
       </c>
       <c r="E11" s="34"/>
       <c r="F11" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="G11" s="134" t="s">
+      <c r="G11" s="103" t="s">
         <v>208</v>
       </c>
-      <c r="H11" s="116" t="s">
+      <c r="H11" s="85" t="s">
         <v>207</v>
       </c>
-      <c r="I11" s="117" t="s">
+      <c r="I11" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="J11" s="118" t="s">
+      <c r="J11" s="87" t="s">
         <v>215</v>
       </c>
-      <c r="K11" s="119" t="s">
+      <c r="K11" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="L11" s="119" t="s">
+      <c r="L11" s="88" t="s">
         <v>213</v>
       </c>
-      <c r="M11" s="119" t="s">
+      <c r="M11" s="88" t="s">
         <v>228</v>
       </c>
-      <c r="N11" s="116" t="s">
+      <c r="N11" s="85" t="s">
         <v>220</v>
       </c>
-      <c r="O11" s="117" t="s">
+      <c r="O11" s="86" t="s">
         <v>218</v>
       </c>
-      <c r="P11" s="119" t="s">
+      <c r="P11" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="Q11" s="119" t="s">
+      <c r="Q11" s="88" t="s">
         <v>211</v>
       </c>
-      <c r="R11" s="119" t="s">
+      <c r="R11" s="88" t="s">
         <v>210</v>
       </c>
-      <c r="S11" s="119" t="s">
+      <c r="S11" s="88" t="s">
         <v>229</v>
       </c>
-      <c r="T11" s="120" t="s">
+      <c r="T11" s="89" t="s">
         <v>221</v>
       </c>
       <c r="U11" s="59"/>
@@ -3369,59 +3312,59 @@
       <c r="A12" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="B12" s="210" t="s">
+      <c r="B12" s="154" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="211" t="s">
+      <c r="C12" s="155" t="s">
         <v>157</v>
       </c>
-      <c r="D12" s="212" t="s">
+      <c r="D12" s="156" t="s">
         <v>158</v>
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="G12" s="115" t="s">
+      <c r="G12" s="84" t="s">
         <v>209</v>
       </c>
-      <c r="H12" s="135" t="s">
+      <c r="H12" s="104" t="s">
         <v>208</v>
       </c>
-      <c r="I12" s="117" t="s">
+      <c r="I12" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="J12" s="119" t="s">
+      <c r="J12" s="88" t="s">
         <v>227</v>
       </c>
-      <c r="K12" s="117" t="s">
+      <c r="K12" s="86" t="s">
         <v>215</v>
       </c>
-      <c r="L12" s="119" t="s">
+      <c r="L12" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="M12" s="119" t="s">
+      <c r="M12" s="88" t="s">
         <v>213</v>
       </c>
-      <c r="N12" s="116" t="s">
+      <c r="N12" s="85" t="s">
         <v>228</v>
       </c>
-      <c r="O12" s="117" t="s">
+      <c r="O12" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="P12" s="119" t="s">
+      <c r="P12" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="Q12" s="119" t="s">
+      <c r="Q12" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="R12" s="119" t="s">
+      <c r="R12" s="88" t="s">
         <v>211</v>
       </c>
-      <c r="S12" s="119" t="s">
+      <c r="S12" s="88" t="s">
         <v>210</v>
       </c>
-      <c r="T12" s="120" t="s">
+      <c r="T12" s="89" t="s">
         <v>229</v>
       </c>
       <c r="U12" s="59"/>
@@ -3445,57 +3388,57 @@
       <c r="A13" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="217"/>
-      <c r="C13" s="211" t="s">
+      <c r="B13" s="161"/>
+      <c r="C13" s="155" t="s">
         <v>159</v>
       </c>
-      <c r="D13" s="212" t="s">
+      <c r="D13" s="156" t="s">
         <v>160</v>
       </c>
       <c r="E13" s="34"/>
       <c r="F13" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="G13" s="115" t="s">
+      <c r="G13" s="84" t="s">
         <v>230</v>
       </c>
-      <c r="H13" s="116" t="s">
+      <c r="H13" s="85" t="s">
         <v>209</v>
       </c>
-      <c r="I13" s="136" t="s">
+      <c r="I13" s="105" t="s">
         <v>208</v>
       </c>
-      <c r="J13" s="119" t="s">
+      <c r="J13" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="K13" s="119" t="s">
+      <c r="K13" s="88" t="s">
         <v>227</v>
       </c>
-      <c r="L13" s="119" t="s">
+      <c r="L13" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="M13" s="119" t="s">
+      <c r="M13" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="N13" s="116" t="s">
+      <c r="N13" s="85" t="s">
         <v>213</v>
       </c>
-      <c r="O13" s="117" t="s">
+      <c r="O13" s="86" t="s">
         <v>228</v>
       </c>
-      <c r="P13" s="119" t="s">
+      <c r="P13" s="88" t="s">
         <v>220</v>
       </c>
-      <c r="Q13" s="119" t="s">
+      <c r="Q13" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="R13" s="119" t="s">
+      <c r="R13" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="S13" s="119" t="s">
+      <c r="S13" s="88" t="s">
         <v>211</v>
       </c>
-      <c r="T13" s="120" t="s">
+      <c r="T13" s="89" t="s">
         <v>210</v>
       </c>
       <c r="U13" s="59"/>
@@ -3519,59 +3462,59 @@
       <c r="A14" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="B14" s="210" t="s">
+      <c r="B14" s="154" t="s">
         <v>161</v>
       </c>
-      <c r="C14" s="211" t="s">
+      <c r="C14" s="155" t="s">
         <v>162</v>
       </c>
-      <c r="D14" s="212" t="s">
+      <c r="D14" s="156" t="s">
         <v>163</v>
       </c>
       <c r="E14" s="34"/>
       <c r="F14" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="G14" s="115" t="s">
+      <c r="G14" s="84" t="s">
         <v>221</v>
       </c>
-      <c r="H14" s="116" t="s">
+      <c r="H14" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="I14" s="117" t="s">
+      <c r="I14" s="86" t="s">
         <v>209</v>
       </c>
-      <c r="J14" s="137" t="s">
+      <c r="J14" s="106" t="s">
         <v>208</v>
       </c>
-      <c r="K14" s="119" t="s">
+      <c r="K14" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="L14" s="119" t="s">
+      <c r="L14" s="88" t="s">
         <v>227</v>
       </c>
-      <c r="M14" s="119" t="s">
+      <c r="M14" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="N14" s="116" t="s">
+      <c r="N14" s="85" t="s">
         <v>214</v>
       </c>
-      <c r="O14" s="117" t="s">
+      <c r="O14" s="86" t="s">
         <v>213</v>
       </c>
-      <c r="P14" s="119" t="s">
+      <c r="P14" s="88" t="s">
         <v>228</v>
       </c>
-      <c r="Q14" s="119" t="s">
+      <c r="Q14" s="88" t="s">
         <v>220</v>
       </c>
-      <c r="R14" s="119" t="s">
+      <c r="R14" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="S14" s="119" t="s">
+      <c r="S14" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="T14" s="120" t="s">
+      <c r="T14" s="89" t="s">
         <v>211</v>
       </c>
       <c r="U14" s="59"/>
@@ -3595,59 +3538,59 @@
       <c r="A15" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B15" s="210" t="s">
+      <c r="B15" s="154" t="s">
         <v>164</v>
       </c>
-      <c r="C15" s="211" t="s">
+      <c r="C15" s="155" t="s">
         <v>165</v>
       </c>
-      <c r="D15" s="212" t="s">
+      <c r="D15" s="156" t="s">
         <v>166</v>
       </c>
       <c r="E15" s="34"/>
       <c r="F15" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="G15" s="115" t="s">
+      <c r="G15" s="84" t="s">
         <v>229</v>
       </c>
-      <c r="H15" s="116" t="s">
+      <c r="H15" s="85" t="s">
         <v>221</v>
       </c>
-      <c r="I15" s="117" t="s">
+      <c r="I15" s="86" t="s">
         <v>230</v>
       </c>
-      <c r="J15" s="119" t="s">
+      <c r="J15" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="K15" s="137" t="s">
+      <c r="K15" s="106" t="s">
         <v>208</v>
       </c>
-      <c r="L15" s="119" t="s">
+      <c r="L15" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="M15" s="119" t="s">
+      <c r="M15" s="88" t="s">
         <v>227</v>
       </c>
-      <c r="N15" s="116" t="s">
+      <c r="N15" s="85" t="s">
         <v>215</v>
       </c>
-      <c r="O15" s="117" t="s">
+      <c r="O15" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="P15" s="119" t="s">
+      <c r="P15" s="88" t="s">
         <v>213</v>
       </c>
-      <c r="Q15" s="119" t="s">
+      <c r="Q15" s="88" t="s">
         <v>228</v>
       </c>
-      <c r="R15" s="119" t="s">
+      <c r="R15" s="88" t="s">
         <v>220</v>
       </c>
-      <c r="S15" s="119" t="s">
+      <c r="S15" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="T15" s="120" t="s">
+      <c r="T15" s="89" t="s">
         <v>212</v>
       </c>
       <c r="U15" s="59"/>
@@ -3671,57 +3614,57 @@
       <c r="A16" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="B16" s="210" t="s">
+      <c r="B16" s="154" t="s">
         <v>167</v>
       </c>
-      <c r="C16" s="211" t="s">
+      <c r="C16" s="155" t="s">
         <v>168</v>
       </c>
-      <c r="D16" s="216"/>
+      <c r="D16" s="160"/>
       <c r="E16" s="34"/>
       <c r="F16" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="G16" s="115" t="s">
+      <c r="G16" s="84" t="s">
         <v>210</v>
       </c>
-      <c r="H16" s="116" t="s">
+      <c r="H16" s="85" t="s">
         <v>229</v>
       </c>
-      <c r="I16" s="117" t="s">
+      <c r="I16" s="86" t="s">
         <v>221</v>
       </c>
-      <c r="J16" s="119" t="s">
+      <c r="J16" s="88" t="s">
         <v>230</v>
       </c>
-      <c r="K16" s="119" t="s">
+      <c r="K16" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="L16" s="137" t="s">
+      <c r="L16" s="106" t="s">
         <v>208</v>
       </c>
-      <c r="M16" s="119" t="s">
+      <c r="M16" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="N16" s="116" t="s">
+      <c r="N16" s="85" t="s">
         <v>227</v>
       </c>
-      <c r="O16" s="117" t="s">
+      <c r="O16" s="86" t="s">
         <v>215</v>
       </c>
-      <c r="P16" s="119" t="s">
+      <c r="P16" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="Q16" s="119" t="s">
+      <c r="Q16" s="88" t="s">
         <v>213</v>
       </c>
-      <c r="R16" s="119" t="s">
+      <c r="R16" s="88" t="s">
         <v>228</v>
       </c>
-      <c r="S16" s="119" t="s">
+      <c r="S16" s="88" t="s">
         <v>220</v>
       </c>
-      <c r="T16" s="120" t="s">
+      <c r="T16" s="89" t="s">
         <v>218</v>
       </c>
       <c r="U16" s="59"/>
@@ -3745,59 +3688,59 @@
       <c r="A17" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="B17" s="210" t="s">
+      <c r="B17" s="154" t="s">
         <v>169</v>
       </c>
-      <c r="C17" s="211" t="s">
+      <c r="C17" s="155" t="s">
         <v>170</v>
       </c>
-      <c r="D17" s="212" t="s">
+      <c r="D17" s="156" t="s">
         <v>171</v>
       </c>
       <c r="E17" s="34"/>
       <c r="F17" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="G17" s="121" t="s">
+      <c r="G17" s="90" t="s">
         <v>211</v>
       </c>
-      <c r="H17" s="116" t="s">
+      <c r="H17" s="85" t="s">
         <v>210</v>
       </c>
-      <c r="I17" s="117" t="s">
+      <c r="I17" s="86" t="s">
         <v>229</v>
       </c>
-      <c r="J17" s="119" t="s">
+      <c r="J17" s="88" t="s">
         <v>221</v>
       </c>
-      <c r="K17" s="119" t="s">
+      <c r="K17" s="88" t="s">
         <v>230</v>
       </c>
-      <c r="L17" s="119" t="s">
+      <c r="L17" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="M17" s="137" t="s">
+      <c r="M17" s="106" t="s">
         <v>208</v>
       </c>
-      <c r="N17" s="116" t="s">
+      <c r="N17" s="85" t="s">
         <v>207</v>
       </c>
-      <c r="O17" s="117" t="s">
+      <c r="O17" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="P17" s="119" t="s">
+      <c r="P17" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="Q17" s="119" t="s">
+      <c r="Q17" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="R17" s="119" t="s">
+      <c r="R17" s="88" t="s">
         <v>213</v>
       </c>
-      <c r="S17" s="119" t="s">
+      <c r="S17" s="88" t="s">
         <v>228</v>
       </c>
-      <c r="T17" s="120" t="s">
+      <c r="T17" s="89" t="s">
         <v>220</v>
       </c>
       <c r="U17" s="59"/>
@@ -3821,57 +3764,57 @@
       <c r="A18" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="B18" s="217" t="s">
+      <c r="B18" s="161" t="s">
         <v>172</v>
       </c>
-      <c r="C18" s="218" t="s">
+      <c r="C18" s="162" t="s">
         <v>173</v>
       </c>
-      <c r="D18" s="212"/>
+      <c r="D18" s="156"/>
       <c r="E18" s="34"/>
       <c r="F18" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="G18" s="115" t="s">
+      <c r="G18" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="H18" s="116" t="s">
+      <c r="H18" s="85" t="s">
         <v>231</v>
       </c>
-      <c r="I18" s="117" t="s">
+      <c r="I18" s="86" t="s">
         <v>210</v>
       </c>
-      <c r="J18" s="119" t="s">
+      <c r="J18" s="88" t="s">
         <v>229</v>
       </c>
-      <c r="K18" s="119" t="s">
+      <c r="K18" s="88" t="s">
         <v>221</v>
       </c>
-      <c r="L18" s="119" t="s">
+      <c r="L18" s="88" t="s">
         <v>232</v>
       </c>
-      <c r="M18" s="119" t="s">
+      <c r="M18" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="N18" s="135" t="s">
+      <c r="N18" s="104" t="s">
         <v>208</v>
       </c>
-      <c r="O18" s="117" t="s">
+      <c r="O18" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="P18" s="119" t="s">
+      <c r="P18" s="88" t="s">
         <v>216</v>
       </c>
-      <c r="Q18" s="119" t="s">
+      <c r="Q18" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="R18" s="119" t="s">
+      <c r="R18" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="S18" s="119" t="s">
+      <c r="S18" s="88" t="s">
         <v>213</v>
       </c>
-      <c r="T18" s="120" t="s">
+      <c r="T18" s="89" t="s">
         <v>219</v>
       </c>
       <c r="U18" s="64"/>
@@ -3895,59 +3838,59 @@
       <c r="A19" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="B19" s="210" t="s">
+      <c r="B19" s="154" t="s">
         <v>174</v>
       </c>
-      <c r="C19" s="211" t="s">
+      <c r="C19" s="155" t="s">
         <v>175</v>
       </c>
-      <c r="D19" s="212" t="s">
+      <c r="D19" s="156" t="s">
         <v>176</v>
       </c>
       <c r="E19" s="34"/>
       <c r="F19" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="G19" s="115" t="s">
+      <c r="G19" s="84" t="s">
         <v>218</v>
       </c>
-      <c r="H19" s="116" t="s">
+      <c r="H19" s="85" t="s">
         <v>212</v>
       </c>
-      <c r="I19" s="117" t="s">
+      <c r="I19" s="86" t="s">
         <v>231</v>
       </c>
-      <c r="J19" s="119" t="s">
+      <c r="J19" s="88" t="s">
         <v>210</v>
       </c>
-      <c r="K19" s="119" t="s">
+      <c r="K19" s="88" t="s">
         <v>229</v>
       </c>
-      <c r="L19" s="119" t="s">
+      <c r="L19" s="88" t="s">
         <v>221</v>
       </c>
-      <c r="M19" s="119" t="s">
+      <c r="M19" s="88" t="s">
         <v>232</v>
       </c>
-      <c r="N19" s="129" t="s">
+      <c r="N19" s="98" t="s">
         <v>209</v>
       </c>
-      <c r="O19" s="117" t="s">
+      <c r="O19" s="86" t="s">
         <v>208</v>
       </c>
-      <c r="P19" s="119" t="s">
+      <c r="P19" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="Q19" s="119" t="s">
+      <c r="Q19" s="88" t="s">
         <v>216</v>
       </c>
-      <c r="R19" s="119" t="s">
+      <c r="R19" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="S19" s="119" t="s">
+      <c r="S19" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="T19" s="120" t="s">
+      <c r="T19" s="89" t="s">
         <v>213</v>
       </c>
       <c r="U19" s="59"/>
@@ -3971,59 +3914,59 @@
       <c r="A20" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="B20" s="210" t="s">
+      <c r="B20" s="154" t="s">
         <v>177</v>
       </c>
-      <c r="C20" s="211" t="s">
+      <c r="C20" s="155" t="s">
         <v>178</v>
       </c>
-      <c r="D20" s="212" t="s">
+      <c r="D20" s="156" t="s">
         <v>179</v>
       </c>
       <c r="E20" s="34"/>
       <c r="F20" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="133" t="s">
+      <c r="G20" s="102" t="s">
         <v>220</v>
       </c>
-      <c r="H20" s="116" t="s">
+      <c r="H20" s="85" t="s">
         <v>218</v>
       </c>
-      <c r="I20" s="117" t="s">
+      <c r="I20" s="86" t="s">
         <v>212</v>
       </c>
-      <c r="J20" s="119" t="s">
+      <c r="J20" s="88" t="s">
         <v>231</v>
       </c>
-      <c r="K20" s="119" t="s">
+      <c r="K20" s="88" t="s">
         <v>210</v>
       </c>
-      <c r="L20" s="119" t="s">
+      <c r="L20" s="88" t="s">
         <v>229</v>
       </c>
-      <c r="M20" s="119" t="s">
+      <c r="M20" s="88" t="s">
         <v>221</v>
       </c>
-      <c r="N20" s="116" t="s">
+      <c r="N20" s="85" t="s">
         <v>232</v>
       </c>
-      <c r="O20" s="117" t="s">
+      <c r="O20" s="86" t="s">
         <v>209</v>
       </c>
-      <c r="P20" s="119" t="s">
+      <c r="P20" s="88" t="s">
         <v>208</v>
       </c>
-      <c r="Q20" s="119" t="s">
+      <c r="Q20" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="R20" s="119" t="s">
+      <c r="R20" s="88" t="s">
         <v>216</v>
       </c>
-      <c r="S20" s="119" t="s">
+      <c r="S20" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="T20" s="120" t="s">
+      <c r="T20" s="89" t="s">
         <v>214</v>
       </c>
       <c r="U20" s="59"/>
@@ -4047,59 +3990,59 @@
       <c r="A21" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="B21" s="210" t="s">
+      <c r="B21" s="154" t="s">
         <v>180</v>
       </c>
-      <c r="C21" s="211" t="s">
+      <c r="C21" s="155" t="s">
         <v>181</v>
       </c>
-      <c r="D21" s="212" t="s">
+      <c r="D21" s="156" t="s">
         <v>182</v>
       </c>
       <c r="E21" s="34"/>
       <c r="F21" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="G21" s="121" t="s">
+      <c r="G21" s="90" t="s">
         <v>219</v>
       </c>
-      <c r="H21" s="129" t="s">
+      <c r="H21" s="98" t="s">
         <v>220</v>
       </c>
-      <c r="I21" s="117" t="s">
+      <c r="I21" s="86" t="s">
         <v>218</v>
       </c>
-      <c r="J21" s="119" t="s">
+      <c r="J21" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="K21" s="119" t="s">
+      <c r="K21" s="88" t="s">
         <v>231</v>
       </c>
-      <c r="L21" s="119" t="s">
+      <c r="L21" s="88" t="s">
         <v>210</v>
       </c>
-      <c r="M21" s="119" t="s">
+      <c r="M21" s="88" t="s">
         <v>229</v>
       </c>
-      <c r="N21" s="116" t="s">
+      <c r="N21" s="85" t="s">
         <v>221</v>
       </c>
-      <c r="O21" s="117" t="s">
+      <c r="O21" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="P21" s="119" t="s">
+      <c r="P21" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="Q21" s="119" t="s">
+      <c r="Q21" s="88" t="s">
         <v>208</v>
       </c>
-      <c r="R21" s="119" t="s">
+      <c r="R21" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="S21" s="119" t="s">
+      <c r="S21" s="88" t="s">
         <v>216</v>
       </c>
-      <c r="T21" s="120" t="s">
+      <c r="T21" s="89" t="s">
         <v>215</v>
       </c>
       <c r="U21" s="59"/>
@@ -4123,59 +4066,59 @@
       <c r="A22" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="B22" s="210" t="s">
+      <c r="B22" s="154" t="s">
         <v>183</v>
       </c>
-      <c r="C22" s="211" t="s">
+      <c r="C22" s="155" t="s">
         <v>184</v>
       </c>
-      <c r="D22" s="212" t="s">
+      <c r="D22" s="156" t="s">
         <v>185</v>
       </c>
       <c r="E22" s="34"/>
       <c r="F22" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="G22" s="115" t="s">
+      <c r="G22" s="84" t="s">
         <v>213</v>
       </c>
-      <c r="H22" s="116" t="s">
+      <c r="H22" s="85" t="s">
         <v>219</v>
       </c>
-      <c r="I22" s="132" t="s">
+      <c r="I22" s="101" t="s">
         <v>220</v>
       </c>
-      <c r="J22" s="119" t="s">
+      <c r="J22" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="K22" s="119" t="s">
+      <c r="K22" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="L22" s="119" t="s">
+      <c r="L22" s="88" t="s">
         <v>231</v>
       </c>
-      <c r="M22" s="119" t="s">
+      <c r="M22" s="88" t="s">
         <v>210</v>
       </c>
-      <c r="N22" s="116" t="s">
+      <c r="N22" s="85" t="s">
         <v>229</v>
       </c>
-      <c r="O22" s="117" t="s">
+      <c r="O22" s="86" t="s">
         <v>221</v>
       </c>
-      <c r="P22" s="119" t="s">
+      <c r="P22" s="88" t="s">
         <v>232</v>
       </c>
-      <c r="Q22" s="119" t="s">
+      <c r="Q22" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="R22" s="119" t="s">
+      <c r="R22" s="88" t="s">
         <v>208</v>
       </c>
-      <c r="S22" s="119" t="s">
+      <c r="S22" s="88" t="s">
         <v>207</v>
       </c>
-      <c r="T22" s="120" t="s">
+      <c r="T22" s="89" t="s">
         <v>216</v>
       </c>
       <c r="U22" s="59"/>
@@ -4199,59 +4142,59 @@
       <c r="A23" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="B23" s="210" t="s">
+      <c r="B23" s="154" t="s">
         <v>186</v>
       </c>
-      <c r="C23" s="211" t="s">
+      <c r="C23" s="155" t="s">
         <v>187</v>
       </c>
-      <c r="D23" s="212" t="s">
+      <c r="D23" s="156" t="s">
         <v>188</v>
       </c>
       <c r="E23" s="34"/>
       <c r="F23" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="115" t="s">
+      <c r="G23" s="84" t="s">
         <v>214</v>
       </c>
-      <c r="H23" s="116" t="s">
+      <c r="H23" s="85" t="s">
         <v>213</v>
       </c>
-      <c r="I23" s="117" t="s">
+      <c r="I23" s="86" t="s">
         <v>219</v>
       </c>
-      <c r="J23" s="130" t="s">
+      <c r="J23" s="99" t="s">
         <v>220</v>
       </c>
-      <c r="K23" s="119" t="s">
+      <c r="K23" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="L23" s="119" t="s">
+      <c r="L23" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="M23" s="119" t="s">
+      <c r="M23" s="88" t="s">
         <v>231</v>
       </c>
-      <c r="N23" s="116" t="s">
+      <c r="N23" s="85" t="s">
         <v>210</v>
       </c>
-      <c r="O23" s="117" t="s">
+      <c r="O23" s="86" t="s">
         <v>229</v>
       </c>
-      <c r="P23" s="119" t="s">
+      <c r="P23" s="88" t="s">
         <v>221</v>
       </c>
-      <c r="Q23" s="119" t="s">
+      <c r="Q23" s="88" t="s">
         <v>232</v>
       </c>
-      <c r="R23" s="119" t="s">
+      <c r="R23" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="S23" s="119" t="s">
+      <c r="S23" s="88" t="s">
         <v>208</v>
       </c>
-      <c r="T23" s="120" t="s">
+      <c r="T23" s="89" t="s">
         <v>207</v>
       </c>
       <c r="U23" s="59"/>
@@ -4275,59 +4218,59 @@
       <c r="A24" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B24" s="210" t="s">
+      <c r="B24" s="154" t="s">
         <v>189</v>
       </c>
-      <c r="C24" s="211" t="s">
+      <c r="C24" s="155" t="s">
         <v>190</v>
       </c>
-      <c r="D24" s="212" t="s">
+      <c r="D24" s="156" t="s">
         <v>191</v>
       </c>
       <c r="E24" s="34"/>
       <c r="F24" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="G24" s="115" t="s">
+      <c r="G24" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="H24" s="116" t="s">
+      <c r="H24" s="85" t="s">
         <v>214</v>
       </c>
-      <c r="I24" s="117" t="s">
+      <c r="I24" s="86" t="s">
         <v>213</v>
       </c>
-      <c r="J24" s="119" t="s">
+      <c r="J24" s="88" t="s">
         <v>219</v>
       </c>
-      <c r="K24" s="130" t="s">
+      <c r="K24" s="99" t="s">
         <v>220</v>
       </c>
-      <c r="L24" s="119" t="s">
+      <c r="L24" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="M24" s="119" t="s">
+      <c r="M24" s="88" t="s">
         <v>212</v>
       </c>
-      <c r="N24" s="116" t="s">
+      <c r="N24" s="85" t="s">
         <v>231</v>
       </c>
-      <c r="O24" s="117" t="s">
+      <c r="O24" s="86" t="s">
         <v>210</v>
       </c>
-      <c r="P24" s="119" t="s">
+      <c r="P24" s="88" t="s">
         <v>229</v>
       </c>
-      <c r="Q24" s="119" t="s">
+      <c r="Q24" s="88" t="s">
         <v>221</v>
       </c>
-      <c r="R24" s="119" t="s">
+      <c r="R24" s="88" t="s">
         <v>232</v>
       </c>
-      <c r="S24" s="119" t="s">
+      <c r="S24" s="88" t="s">
         <v>209</v>
       </c>
-      <c r="T24" s="120" t="s">
+      <c r="T24" s="89" t="s">
         <v>208</v>
       </c>
       <c r="U24" s="59"/>
@@ -4351,59 +4294,59 @@
       <c r="A25" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="213" t="s">
+      <c r="B25" s="157" t="s">
         <v>192</v>
       </c>
-      <c r="C25" s="214" t="s">
+      <c r="C25" s="158" t="s">
         <v>193</v>
       </c>
-      <c r="D25" s="215" t="s">
+      <c r="D25" s="159" t="s">
         <v>194</v>
       </c>
       <c r="E25" s="34"/>
       <c r="F25" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="G25" s="122" t="s">
+      <c r="G25" s="91" t="s">
         <v>216</v>
       </c>
-      <c r="H25" s="123" t="s">
+      <c r="H25" s="92" t="s">
         <v>215</v>
       </c>
-      <c r="I25" s="124" t="s">
+      <c r="I25" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="J25" s="125" t="s">
+      <c r="J25" s="94" t="s">
         <v>213</v>
       </c>
-      <c r="K25" s="125" t="s">
+      <c r="K25" s="94" t="s">
         <v>219</v>
       </c>
-      <c r="L25" s="131" t="s">
+      <c r="L25" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="M25" s="125" t="s">
+      <c r="M25" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="N25" s="123" t="s">
+      <c r="N25" s="92" t="s">
         <v>212</v>
       </c>
-      <c r="O25" s="124" t="s">
+      <c r="O25" s="93" t="s">
         <v>231</v>
       </c>
-      <c r="P25" s="125" t="s">
+      <c r="P25" s="94" t="s">
         <v>210</v>
       </c>
-      <c r="Q25" s="125" t="s">
+      <c r="Q25" s="94" t="s">
         <v>229</v>
       </c>
-      <c r="R25" s="125" t="s">
+      <c r="R25" s="94" t="s">
         <v>221</v>
       </c>
-      <c r="S25" s="125" t="s">
+      <c r="S25" s="94" t="s">
         <v>232</v>
       </c>
-      <c r="T25" s="126" t="s">
+      <c r="T25" s="95" t="s">
         <v>209</v>
       </c>
       <c r="U25" s="62"/>
@@ -4478,48 +4421,48 @@
       <c r="AG28" s="5"/>
     </row>
     <row r="29" spans="1:39" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="169" t="s">
         <v>198</v>
       </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="68"/>
-      <c r="H29" s="66" t="s">
+      <c r="C29" s="170"/>
+      <c r="D29" s="170"/>
+      <c r="E29" s="171"/>
+      <c r="H29" s="169" t="s">
         <v>152</v>
       </c>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="L29" s="67"/>
-      <c r="M29" s="68"/>
+      <c r="I29" s="170"/>
+      <c r="J29" s="170"/>
+      <c r="K29" s="170"/>
+      <c r="L29" s="170"/>
+      <c r="M29" s="171"/>
       <c r="O29" s="52"/>
-      <c r="P29" s="66" t="s">
+      <c r="P29" s="169" t="s">
         <v>153</v>
       </c>
-      <c r="Q29" s="67"/>
-      <c r="R29" s="67"/>
-      <c r="S29" s="67"/>
-      <c r="T29" s="67"/>
-      <c r="U29" s="68"/>
+      <c r="Q29" s="170"/>
+      <c r="R29" s="170"/>
+      <c r="S29" s="170"/>
+      <c r="T29" s="170"/>
+      <c r="U29" s="171"/>
     </row>
     <row r="30" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="69"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="70"/>
-      <c r="K30" s="70"/>
-      <c r="L30" s="70"/>
-      <c r="M30" s="71"/>
+      <c r="B30" s="172"/>
+      <c r="C30" s="173"/>
+      <c r="D30" s="173"/>
+      <c r="E30" s="174"/>
+      <c r="H30" s="172"/>
+      <c r="I30" s="173"/>
+      <c r="J30" s="173"/>
+      <c r="K30" s="173"/>
+      <c r="L30" s="173"/>
+      <c r="M30" s="174"/>
       <c r="O30" s="52"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="70"/>
-      <c r="R30" s="70"/>
-      <c r="S30" s="70"/>
-      <c r="T30" s="70"/>
-      <c r="U30" s="71"/>
+      <c r="P30" s="172"/>
+      <c r="Q30" s="173"/>
+      <c r="R30" s="173"/>
+      <c r="S30" s="173"/>
+      <c r="T30" s="173"/>
+      <c r="U30" s="174"/>
     </row>
     <row r="31" spans="1:39" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="31"/>
@@ -4557,39 +4500,39 @@
       </c>
     </row>
     <row r="32" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="78" t="s">
+      <c r="B32" s="190" t="s">
         <v>199</v>
       </c>
-      <c r="C32" s="79"/>
-      <c r="D32" s="79"/>
-      <c r="E32" s="80"/>
-      <c r="H32" s="138" t="s">
+      <c r="C32" s="191"/>
+      <c r="D32" s="191"/>
+      <c r="E32" s="192"/>
+      <c r="H32" s="107" t="s">
         <v>111</v>
       </c>
-      <c r="I32" s="139"/>
-      <c r="J32" s="140" t="s">
+      <c r="I32" s="108"/>
+      <c r="J32" s="109" t="s">
         <v>94</v>
       </c>
-      <c r="K32" s="141"/>
-      <c r="L32" s="142" t="s">
+      <c r="K32" s="110"/>
+      <c r="L32" s="111" t="s">
         <v>99</v>
       </c>
-      <c r="M32" s="143" t="s">
+      <c r="M32" s="112" t="s">
         <v>113</v>
       </c>
       <c r="O32" s="51"/>
-      <c r="P32" s="172" t="s">
+      <c r="P32" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="Q32" s="173"/>
-      <c r="R32" s="172" t="s">
+      <c r="Q32" s="110"/>
+      <c r="R32" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="S32" s="173"/>
-      <c r="T32" s="174" t="s">
+      <c r="S32" s="110"/>
+      <c r="T32" s="137" t="s">
         <v>72</v>
       </c>
-      <c r="U32" s="175" t="s">
+      <c r="U32" s="138" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4598,105 +4541,105 @@
       <c r="C33" s="43"/>
       <c r="D33" s="43"/>
       <c r="E33" s="44"/>
-      <c r="H33" s="144" t="s">
+      <c r="H33" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="145"/>
-      <c r="J33" s="146" t="s">
+      <c r="I33" s="114"/>
+      <c r="J33" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="K33" s="147"/>
-      <c r="L33" s="148" t="s">
+      <c r="K33" s="116"/>
+      <c r="L33" s="117" t="s">
         <v>100</v>
       </c>
-      <c r="M33" s="149" t="s">
+      <c r="M33" s="118" t="s">
         <v>114</v>
       </c>
       <c r="O33" s="51"/>
-      <c r="P33" s="176" t="s">
+      <c r="P33" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="Q33" s="177"/>
-      <c r="R33" s="176" t="s">
+      <c r="Q33" s="116"/>
+      <c r="R33" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="S33" s="177"/>
-      <c r="T33" s="178" t="s">
+      <c r="S33" s="116"/>
+      <c r="T33" s="139" t="s">
         <v>73</v>
       </c>
-      <c r="U33" s="179" t="s">
+      <c r="U33" s="140" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="34" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="190" t="s">
         <v>217</v>
       </c>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="80"/>
-      <c r="H34" s="144" t="s">
+      <c r="C34" s="191"/>
+      <c r="D34" s="191"/>
+      <c r="E34" s="192"/>
+      <c r="H34" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="I34" s="145"/>
-      <c r="J34" s="146" t="s">
+      <c r="I34" s="114"/>
+      <c r="J34" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="K34" s="147"/>
-      <c r="L34" s="148" t="s">
+      <c r="K34" s="116"/>
+      <c r="L34" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="M34" s="149" t="s">
+      <c r="M34" s="118" t="s">
         <v>115</v>
       </c>
       <c r="O34" s="51"/>
-      <c r="P34" s="176" t="s">
+      <c r="P34" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="Q34" s="177"/>
-      <c r="R34" s="176" t="s">
+      <c r="Q34" s="116"/>
+      <c r="R34" s="115" t="s">
         <v>202</v>
       </c>
-      <c r="S34" s="177"/>
-      <c r="T34" s="178" t="s">
+      <c r="S34" s="116"/>
+      <c r="T34" s="139" t="s">
         <v>74</v>
       </c>
-      <c r="U34" s="179" t="s">
+      <c r="U34" s="140" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="35" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="78"/>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="80"/>
-      <c r="H35" s="144" t="s">
+      <c r="B35" s="190"/>
+      <c r="C35" s="191"/>
+      <c r="D35" s="191"/>
+      <c r="E35" s="192"/>
+      <c r="H35" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="I35" s="145"/>
-      <c r="J35" s="146" t="s">
+      <c r="I35" s="114"/>
+      <c r="J35" s="115" t="s">
         <v>121</v>
       </c>
-      <c r="K35" s="147"/>
-      <c r="L35" s="148" t="s">
+      <c r="K35" s="116"/>
+      <c r="L35" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="M35" s="149" t="s">
+      <c r="M35" s="118" t="s">
         <v>225</v>
       </c>
       <c r="O35" s="51"/>
-      <c r="P35" s="176" t="s">
+      <c r="P35" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="Q35" s="177"/>
-      <c r="R35" s="176" t="s">
+      <c r="Q35" s="116"/>
+      <c r="R35" s="115" t="s">
         <v>203</v>
       </c>
-      <c r="S35" s="177"/>
-      <c r="T35" s="178" t="s">
+      <c r="S35" s="116"/>
+      <c r="T35" s="139" t="s">
         <v>75</v>
       </c>
-      <c r="U35" s="179" t="s">
+      <c r="U35" s="140" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4705,105 +4648,105 @@
       <c r="C36" s="43"/>
       <c r="D36" s="43"/>
       <c r="E36" s="44"/>
-      <c r="H36" s="144" t="s">
+      <c r="H36" s="113" t="s">
         <v>112</v>
       </c>
-      <c r="I36" s="145"/>
-      <c r="J36" s="146" t="s">
+      <c r="I36" s="114"/>
+      <c r="J36" s="115" t="s">
         <v>203</v>
       </c>
-      <c r="K36" s="147"/>
-      <c r="L36" s="148" t="s">
+      <c r="K36" s="116"/>
+      <c r="L36" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="M36" s="149" t="s">
+      <c r="M36" s="118" t="s">
         <v>116</v>
       </c>
       <c r="O36" s="51"/>
-      <c r="P36" s="176" t="s">
+      <c r="P36" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="Q36" s="177"/>
-      <c r="R36" s="176" t="s">
+      <c r="Q36" s="116"/>
+      <c r="R36" s="115" t="s">
         <v>118</v>
       </c>
-      <c r="S36" s="177"/>
-      <c r="T36" s="178" t="s">
+      <c r="S36" s="116"/>
+      <c r="T36" s="139" t="s">
         <v>76</v>
       </c>
-      <c r="U36" s="179" t="s">
+      <c r="U36" s="140" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="37" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="78" t="s">
+      <c r="B37" s="190" t="s">
         <v>206</v>
       </c>
-      <c r="C37" s="79"/>
-      <c r="D37" s="79"/>
-      <c r="E37" s="80"/>
-      <c r="H37" s="144" t="s">
+      <c r="C37" s="191"/>
+      <c r="D37" s="191"/>
+      <c r="E37" s="192"/>
+      <c r="H37" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="I37" s="145"/>
-      <c r="J37" s="146" t="s">
+      <c r="I37" s="114"/>
+      <c r="J37" s="115" t="s">
         <v>120</v>
       </c>
-      <c r="K37" s="147"/>
-      <c r="L37" s="148" t="s">
+      <c r="K37" s="116"/>
+      <c r="L37" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="M37" s="149" t="s">
+      <c r="M37" s="118" t="s">
         <v>117</v>
       </c>
       <c r="O37" s="51"/>
-      <c r="P37" s="176" t="s">
+      <c r="P37" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="Q37" s="177"/>
-      <c r="R37" s="176" t="s">
+      <c r="Q37" s="116"/>
+      <c r="R37" s="115" t="s">
         <v>119</v>
       </c>
-      <c r="S37" s="177"/>
-      <c r="T37" s="178" t="s">
+      <c r="S37" s="116"/>
+      <c r="T37" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="U37" s="179" t="s">
+      <c r="U37" s="140" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="38" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="78"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="80"/>
-      <c r="H38" s="144" t="s">
+      <c r="B38" s="190"/>
+      <c r="C38" s="191"/>
+      <c r="D38" s="191"/>
+      <c r="E38" s="192"/>
+      <c r="H38" s="113" t="s">
         <v>111</v>
       </c>
-      <c r="I38" s="145"/>
-      <c r="J38" s="146" t="s">
+      <c r="I38" s="114"/>
+      <c r="J38" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="K38" s="147"/>
-      <c r="L38" s="148" t="s">
+      <c r="K38" s="116"/>
+      <c r="L38" s="117" t="s">
         <v>105</v>
       </c>
-      <c r="M38" s="149" t="s">
+      <c r="M38" s="118" t="s">
         <v>113</v>
       </c>
       <c r="O38" s="51"/>
-      <c r="P38" s="176" t="s">
+      <c r="P38" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="Q38" s="177"/>
-      <c r="R38" s="176" t="s">
+      <c r="Q38" s="116"/>
+      <c r="R38" s="115" t="s">
         <v>121</v>
       </c>
-      <c r="S38" s="177"/>
-      <c r="T38" s="178" t="s">
+      <c r="S38" s="116"/>
+      <c r="T38" s="139" t="s">
         <v>78</v>
       </c>
-      <c r="U38" s="179" t="s">
+      <c r="U38" s="140" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4812,111 +4755,111 @@
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
       <c r="E39" s="47"/>
-      <c r="H39" s="144" t="s">
+      <c r="H39" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="145"/>
-      <c r="J39" s="146" t="s">
+      <c r="I39" s="114"/>
+      <c r="J39" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="K39" s="147"/>
-      <c r="L39" s="148" t="s">
+      <c r="K39" s="116"/>
+      <c r="L39" s="117" t="s">
         <v>106</v>
       </c>
-      <c r="M39" s="149" t="s">
+      <c r="M39" s="118" t="s">
         <v>114</v>
       </c>
       <c r="O39" s="51"/>
-      <c r="P39" s="182" t="s">
+      <c r="P39" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="Q39" s="183"/>
-      <c r="R39" s="182" t="s">
+      <c r="Q39" s="144"/>
+      <c r="R39" s="143" t="s">
         <v>36</v>
       </c>
-      <c r="S39" s="183"/>
-      <c r="T39" s="180" t="s">
+      <c r="S39" s="144"/>
+      <c r="T39" s="141" t="s">
         <v>79</v>
       </c>
-      <c r="U39" s="181" t="s">
+      <c r="U39" s="142" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="40" spans="2:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="78" t="s">
+      <c r="B40" s="190" t="s">
         <v>205</v>
       </c>
-      <c r="C40" s="79"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="80"/>
-      <c r="H40" s="144" t="s">
+      <c r="C40" s="191"/>
+      <c r="D40" s="191"/>
+      <c r="E40" s="192"/>
+      <c r="H40" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="I40" s="145"/>
-      <c r="J40" s="150" t="s">
+      <c r="I40" s="114"/>
+      <c r="J40" s="119" t="s">
         <v>96</v>
       </c>
-      <c r="K40" s="147"/>
-      <c r="L40" s="148" t="s">
+      <c r="K40" s="116"/>
+      <c r="L40" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="M40" s="149" t="s">
+      <c r="M40" s="118" t="s">
         <v>115</v>
       </c>
       <c r="O40" s="52"/>
-      <c r="P40" s="66" t="s">
+      <c r="P40" s="169" t="s">
         <v>154</v>
       </c>
-      <c r="Q40" s="67"/>
-      <c r="R40" s="67"/>
-      <c r="S40" s="67"/>
-      <c r="T40" s="67"/>
-      <c r="U40" s="68"/>
+      <c r="Q40" s="170"/>
+      <c r="R40" s="170"/>
+      <c r="S40" s="170"/>
+      <c r="T40" s="170"/>
+      <c r="U40" s="171"/>
     </row>
     <row r="41" spans="2:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="78"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="80"/>
-      <c r="H41" s="144" t="s">
+      <c r="B41" s="190"/>
+      <c r="C41" s="191"/>
+      <c r="D41" s="191"/>
+      <c r="E41" s="192"/>
+      <c r="H41" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="145"/>
-      <c r="J41" s="146" t="s">
+      <c r="I41" s="114"/>
+      <c r="J41" s="115" t="s">
         <v>119</v>
       </c>
-      <c r="K41" s="147"/>
-      <c r="L41" s="148" t="s">
+      <c r="K41" s="116"/>
+      <c r="L41" s="117" t="s">
         <v>108</v>
       </c>
-      <c r="M41" s="149" t="s">
+      <c r="M41" s="118" t="s">
         <v>225</v>
       </c>
       <c r="O41" s="52"/>
-      <c r="P41" s="69"/>
-      <c r="Q41" s="70"/>
-      <c r="R41" s="70"/>
-      <c r="S41" s="70"/>
-      <c r="T41" s="70"/>
-      <c r="U41" s="71"/>
+      <c r="P41" s="172"/>
+      <c r="Q41" s="173"/>
+      <c r="R41" s="173"/>
+      <c r="S41" s="173"/>
+      <c r="T41" s="173"/>
+      <c r="U41" s="174"/>
     </row>
     <row r="42" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="48"/>
       <c r="C42" s="49"/>
       <c r="D42" s="49"/>
       <c r="E42" s="50"/>
-      <c r="H42" s="144" t="s">
+      <c r="H42" s="113" t="s">
         <v>112</v>
       </c>
-      <c r="I42" s="145"/>
-      <c r="J42" s="146" t="s">
+      <c r="I42" s="114"/>
+      <c r="J42" s="115" t="s">
         <v>118</v>
       </c>
-      <c r="K42" s="147"/>
-      <c r="L42" s="148" t="s">
+      <c r="K42" s="116"/>
+      <c r="L42" s="117" t="s">
         <v>109</v>
       </c>
-      <c r="M42" s="149" t="s">
+      <c r="M42" s="118" t="s">
         <v>116</v>
       </c>
       <c r="O42" s="53"/>
@@ -4936,91 +4879,91 @@
       </c>
     </row>
     <row r="43" spans="2:21" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H43" s="151" t="s">
+      <c r="H43" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="152"/>
-      <c r="J43" s="153" t="s">
+      <c r="I43" s="121"/>
+      <c r="J43" s="122" t="s">
         <v>122</v>
       </c>
-      <c r="K43" s="154"/>
-      <c r="L43" s="155" t="s">
+      <c r="K43" s="123"/>
+      <c r="L43" s="124" t="s">
         <v>110</v>
       </c>
-      <c r="M43" s="156" t="s">
+      <c r="M43" s="125" t="s">
         <v>117</v>
       </c>
       <c r="O43" s="51"/>
-      <c r="P43" s="97" t="s">
+      <c r="P43" s="163" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q43" s="164"/>
+      <c r="R43" s="109" t="s">
+        <v>118</v>
+      </c>
+      <c r="S43" s="110"/>
+      <c r="T43" s="137" t="s">
+        <v>80</v>
+      </c>
+      <c r="U43" s="112" t="s">
         <v>237</v>
       </c>
-      <c r="Q43" s="198"/>
-      <c r="R43" s="184" t="s">
-        <v>118</v>
-      </c>
-      <c r="S43" s="185"/>
-      <c r="T43" s="187" t="s">
-        <v>80</v>
-      </c>
-      <c r="U43" s="186" t="s">
-        <v>238</v>
-      </c>
     </row>
     <row r="44" spans="2:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H44" s="66" t="s">
+      <c r="H44" s="169" t="s">
         <v>155</v>
       </c>
-      <c r="I44" s="67"/>
-      <c r="J44" s="67"/>
-      <c r="K44" s="67"/>
-      <c r="L44" s="67"/>
-      <c r="M44" s="68"/>
+      <c r="I44" s="170"/>
+      <c r="J44" s="170"/>
+      <c r="K44" s="170"/>
+      <c r="L44" s="170"/>
+      <c r="M44" s="171"/>
       <c r="O44" s="51"/>
-      <c r="P44" s="188" t="s">
+      <c r="P44" s="115" t="s">
         <v>123</v>
       </c>
-      <c r="Q44" s="189"/>
-      <c r="R44" s="192" t="s">
+      <c r="Q44" s="116"/>
+      <c r="R44" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="S44" s="189"/>
-      <c r="T44" s="190" t="s">
+      <c r="S44" s="116"/>
+      <c r="T44" s="139" t="s">
         <v>81</v>
       </c>
-      <c r="U44" s="191" t="s">
+      <c r="U44" s="140" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="45" spans="2:21" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H45" s="69"/>
-      <c r="I45" s="70"/>
-      <c r="J45" s="70"/>
-      <c r="K45" s="70"/>
-      <c r="L45" s="70"/>
-      <c r="M45" s="71"/>
+      <c r="H45" s="172"/>
+      <c r="I45" s="173"/>
+      <c r="J45" s="173"/>
+      <c r="K45" s="173"/>
+      <c r="L45" s="173"/>
+      <c r="M45" s="174"/>
       <c r="O45" s="51"/>
-      <c r="P45" s="188" t="s">
+      <c r="P45" s="115" t="s">
         <v>124</v>
       </c>
-      <c r="Q45" s="189"/>
-      <c r="R45" s="188" t="s">
+      <c r="Q45" s="116"/>
+      <c r="R45" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="S45" s="189"/>
-      <c r="T45" s="190" t="s">
+      <c r="S45" s="116"/>
+      <c r="T45" s="139" t="s">
         <v>82</v>
       </c>
-      <c r="U45" s="191" t="s">
+      <c r="U45" s="140" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="46" spans="2:21" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="193" t="s">
         <v>195</v>
       </c>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="74"/>
+      <c r="C46" s="194"/>
+      <c r="D46" s="194"/>
+      <c r="E46" s="195"/>
       <c r="H46" s="26" t="s">
         <v>3</v>
       </c>
@@ -5036,53 +4979,53 @@
         <v>4</v>
       </c>
       <c r="O46" s="51"/>
-      <c r="P46" s="188" t="s">
+      <c r="P46" s="115" t="s">
         <v>125</v>
       </c>
-      <c r="Q46" s="189"/>
-      <c r="R46" s="188" t="s">
+      <c r="Q46" s="116"/>
+      <c r="R46" s="115" t="s">
         <v>204</v>
       </c>
-      <c r="S46" s="189"/>
-      <c r="T46" s="190" t="s">
+      <c r="S46" s="116"/>
+      <c r="T46" s="139" t="s">
         <v>83</v>
       </c>
-      <c r="U46" s="191" t="s">
+      <c r="U46" s="140" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="47" spans="2:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="75"/>
-      <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
-      <c r="E47" s="77"/>
-      <c r="H47" s="157" t="s">
+      <c r="B47" s="196"/>
+      <c r="C47" s="197"/>
+      <c r="D47" s="197"/>
+      <c r="E47" s="198"/>
+      <c r="H47" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="I47" s="161"/>
-      <c r="J47" s="162" t="s">
-        <v>233</v>
-      </c>
-      <c r="K47" s="163"/>
-      <c r="L47" s="158" t="s">
+      <c r="I47" s="126"/>
+      <c r="J47" s="127" t="s">
+        <v>240</v>
+      </c>
+      <c r="K47" s="128"/>
+      <c r="L47" s="112" t="s">
         <v>89</v>
       </c>
-      <c r="M47" s="158" t="s">
+      <c r="M47" s="112" t="s">
         <v>116</v>
       </c>
       <c r="O47" s="51"/>
-      <c r="P47" s="188" t="s">
+      <c r="P47" s="115" t="s">
         <v>123</v>
       </c>
-      <c r="Q47" s="189"/>
-      <c r="R47" s="188" t="s">
+      <c r="Q47" s="116"/>
+      <c r="R47" s="115" t="s">
         <v>94</v>
       </c>
-      <c r="S47" s="189"/>
-      <c r="T47" s="190" t="s">
+      <c r="S47" s="116"/>
+      <c r="T47" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="U47" s="191" t="s">
+      <c r="U47" s="140" t="s">
         <v>226</v>
       </c>
     </row>
@@ -5097,121 +5040,121 @@
       <c r="E48" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="159" t="s">
+      <c r="H48" s="113" t="s">
+        <v>233</v>
+      </c>
+      <c r="I48" s="129"/>
+      <c r="J48" s="130" t="s">
+        <v>240</v>
+      </c>
+      <c r="K48" s="131"/>
+      <c r="L48" s="118" t="s">
+        <v>90</v>
+      </c>
+      <c r="M48" s="118" t="s">
         <v>234</v>
       </c>
-      <c r="I48" s="164"/>
-      <c r="J48" s="165" t="s">
-        <v>233</v>
-      </c>
-      <c r="K48" s="166"/>
-      <c r="L48" s="160" t="s">
-        <v>90</v>
-      </c>
-      <c r="M48" s="160" t="s">
+      <c r="O48" s="51"/>
+      <c r="P48" s="115" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q48" s="116"/>
+      <c r="R48" s="115" t="s">
+        <v>119</v>
+      </c>
+      <c r="S48" s="116"/>
+      <c r="T48" s="139" t="s">
+        <v>85</v>
+      </c>
+      <c r="U48" s="140" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="49" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="165" t="s">
+        <v>196</v>
+      </c>
+      <c r="D49" s="166"/>
+      <c r="E49" s="148" t="s">
+        <v>68</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="H49" s="113" t="s">
+        <v>88</v>
+      </c>
+      <c r="I49" s="129"/>
+      <c r="J49" s="130" t="s">
         <v>235</v>
       </c>
-      <c r="O48" s="51"/>
-      <c r="P48" s="188" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q48" s="189"/>
-      <c r="R48" s="188" t="s">
-        <v>119</v>
-      </c>
-      <c r="S48" s="189"/>
-      <c r="T48" s="190" t="s">
-        <v>85</v>
-      </c>
-      <c r="U48" s="191" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="49" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="202" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="199" t="s">
-        <v>196</v>
-      </c>
-      <c r="D49" s="204"/>
-      <c r="E49" s="200" t="s">
-        <v>68</v>
-      </c>
-      <c r="F49" s="1"/>
-      <c r="H49" s="159" t="s">
-        <v>88</v>
-      </c>
-      <c r="I49" s="164"/>
-      <c r="J49" s="165" t="s">
-        <v>236</v>
-      </c>
-      <c r="K49" s="166"/>
-      <c r="L49" s="160" t="s">
+      <c r="K49" s="131"/>
+      <c r="L49" s="118" t="s">
         <v>91</v>
       </c>
-      <c r="M49" s="160" t="s">
+      <c r="M49" s="118" t="s">
         <v>116</v>
       </c>
       <c r="O49" s="51"/>
-      <c r="P49" s="188" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q49" s="189"/>
-      <c r="R49" s="188" t="s">
+      <c r="P49" s="115" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q49" s="116"/>
+      <c r="R49" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="S49" s="189"/>
-      <c r="T49" s="190" t="s">
+      <c r="S49" s="116"/>
+      <c r="T49" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="U49" s="191" t="s">
+      <c r="U49" s="140" t="s">
         <v>222</v>
       </c>
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
     </row>
     <row r="50" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="203" t="s">
+      <c r="B50" s="150" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="205" t="s">
+      <c r="C50" s="167" t="s">
         <v>197</v>
       </c>
-      <c r="D50" s="206"/>
-      <c r="E50" s="201" t="s">
+      <c r="D50" s="168"/>
+      <c r="E50" s="149" t="s">
         <v>68</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="167" t="s">
+      <c r="H50" s="132" t="s">
+        <v>233</v>
+      </c>
+      <c r="I50" s="133"/>
+      <c r="J50" s="134" t="s">
+        <v>235</v>
+      </c>
+      <c r="K50" s="135"/>
+      <c r="L50" s="136" t="s">
+        <v>92</v>
+      </c>
+      <c r="M50" s="136" t="s">
         <v>234</v>
-      </c>
-      <c r="I50" s="168"/>
-      <c r="J50" s="169" t="s">
-        <v>236</v>
-      </c>
-      <c r="K50" s="170"/>
-      <c r="L50" s="171" t="s">
-        <v>92</v>
-      </c>
-      <c r="M50" s="171" t="s">
-        <v>235</v>
       </c>
       <c r="N50" s="1"/>
       <c r="O50" s="51"/>
-      <c r="P50" s="197" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q50" s="196"/>
-      <c r="R50" s="195" t="s">
+      <c r="P50" s="147" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q50" s="144"/>
+      <c r="R50" s="143" t="s">
         <v>96</v>
       </c>
-      <c r="S50" s="196"/>
-      <c r="T50" s="193" t="s">
+      <c r="S50" s="144"/>
+      <c r="T50" s="145" t="s">
         <v>87</v>
       </c>
-      <c r="U50" s="194" t="s">
+      <c r="U50" s="146" t="s">
         <v>222</v>
       </c>
       <c r="V50" s="1"/>
@@ -5245,17 +5188,17 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="P29:U30"/>
-    <mergeCell ref="P40:U41"/>
     <mergeCell ref="A8:D9"/>
     <mergeCell ref="A1:V4"/>
     <mergeCell ref="G6:V7"/>
     <mergeCell ref="H29:M30"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B29:E30"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="P29:U30"/>
+    <mergeCell ref="P40:U41"/>
     <mergeCell ref="H44:M45"/>
     <mergeCell ref="B46:E47"/>
     <mergeCell ref="B34:E35"/>
@@ -5283,12 +5226,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="199" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">

</xml_diff>